<commit_message>
chore(data): add/update Inputs Excel files
</commit_message>
<xml_diff>
--- a/Inputs/Deskcount/2024/April Deskcount.xlsx
+++ b/Inputs/Deskcount/2024/April Deskcount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greystar365.sharepoint.com/sites/CorporateOfficeStrategy/Shared Documents/General/Occupancy Data/Dashboard/Inputs/Deskcount/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_E35161E09DDAB7BB5CD1F6181239E262265FDBF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEA381BF-18A2-4098-9AD0-C770A7BA6CB1}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_E35161E09DDAB7BB5CD1F6181239E262265FDBF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF480C27-4DC7-4123-8A53-DC7A12AC6AFC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1606,7 +1606,7 @@
         <v>45383</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1686,7 +1686,7 @@
         <v>45383</v>
       </c>
       <c r="F43" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1717,7 +1717,7 @@
         <v>91</v>
       </c>
       <c r="C45" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D45" s="7">
         <v>3509</v>
@@ -1786,7 +1786,7 @@
         <v>45383</v>
       </c>
       <c r="F48" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1806,7 +1806,7 @@
         <v>45383</v>
       </c>
       <c r="F49" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2156,15 +2156,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="247b3ed0-617a-4d1d-b8bd-a66944492619" xsi:nil="true"/>
@@ -2175,19 +2166,35 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE6ABCA9-2ACD-4F05-A87A-5CEA69ED2D90}"/>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74210780-D2ED-4E8B-8299-24F1A344B303}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE6ABCA9-2ACD-4F05-A87A-5CEA69ED2D90}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="334de605-b0fc-4c39-b9f0-ad19cf79a3ca"/>
+    <ds:schemaRef ds:uri="247b3ed0-617a-4d1d-b8bd-a66944492619"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20919586-F825-4328-A511-702B7F6D9530}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2196,4 +2203,12 @@
     <ds:schemaRef ds:uri="334de605-b0fc-4c39-b9f0-ad19cf79a3ca"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74210780-D2ED-4E8B-8299-24F1A344B303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>